<commit_message>
added data for 3mL
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/analysis/printed.xlsx
+++ b/data/commerical-Vs-printed-comparison/analysis/printed.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="2940" windowWidth="20500" windowHeight="8740" tabRatio="500"/>
+    <workbookView xWindow="4820" yWindow="0" windowWidth="21520" windowHeight="12440" tabRatio="758"/>
   </bookViews>
   <sheets>
-    <sheet name="200uL_printed.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="50uL_printed.csv" sheetId="2" r:id="rId2"/>
-    <sheet name="20uL_printed.csv" sheetId="3" r:id="rId3"/>
-    <sheet name="10uL_printed.csv" sheetId="4" r:id="rId4"/>
+    <sheet name="1000uL_printed.csv" sheetId="6" r:id="rId1"/>
+    <sheet name="500uL_printed.csv" sheetId="7" r:id="rId2"/>
+    <sheet name="200uL_printed_3mL.csv" sheetId="8" r:id="rId3"/>
+    <sheet name="300uL_printed.csv" sheetId="5" r:id="rId4"/>
+    <sheet name="200uL_printed.csv" sheetId="1" r:id="rId5"/>
+    <sheet name="50uL_printed.csv" sheetId="2" r:id="rId6"/>
+    <sheet name="20uL_printed.csv" sheetId="3" r:id="rId7"/>
+    <sheet name="10uL_printed.csv" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_10uL_printed" localSheetId="3">'10uL_printed.csv'!$A$1:$C$6</definedName>
-    <definedName name="_200uL_printed" localSheetId="0">'200uL_printed.csv'!$A$1:$C$6</definedName>
-    <definedName name="_20uL_printed" localSheetId="2">'20uL_printed.csv'!$A$1:$C$6</definedName>
-    <definedName name="_50uL_printed" localSheetId="1">'50uL_printed.csv'!$A$1:$C$6</definedName>
+    <definedName name="_10uL_printed" localSheetId="7">'10uL_printed.csv'!$A$1:$C$6</definedName>
+    <definedName name="_200uL_printed" localSheetId="4">'200uL_printed.csv'!$A$1:$C$6</definedName>
+    <definedName name="_20uL_printed" localSheetId="6">'20uL_printed.csv'!$A$1:$C$6</definedName>
+    <definedName name="_50uL_printed" localSheetId="5">'50uL_printed.csv'!$A$1:$C$6</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -69,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>tip1</t>
   </si>
@@ -467,7 +471,351 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>943.8</v>
+      </c>
+      <c r="B2">
+        <v>946.9</v>
+      </c>
+      <c r="C2">
+        <v>947.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>943.5</v>
+      </c>
+      <c r="B3">
+        <v>944.5</v>
+      </c>
+      <c r="C3">
+        <v>947.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>946.6</v>
+      </c>
+      <c r="B4">
+        <v>946.9</v>
+      </c>
+      <c r="C4">
+        <v>944.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>946.9</v>
+      </c>
+      <c r="B5">
+        <v>946.4</v>
+      </c>
+      <c r="C5">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>947.1</v>
+      </c>
+      <c r="B6">
+        <v>947</v>
+      </c>
+      <c r="C6">
+        <v>938.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>475.9</v>
+      </c>
+      <c r="B2">
+        <v>478.5</v>
+      </c>
+      <c r="C2">
+        <v>469.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>473.6</v>
+      </c>
+      <c r="B3">
+        <v>478.9</v>
+      </c>
+      <c r="C3">
+        <v>470.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>474.1</v>
+      </c>
+      <c r="B4">
+        <v>478.3</v>
+      </c>
+      <c r="C4">
+        <v>470.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>473.8</v>
+      </c>
+      <c r="B5">
+        <v>477.8</v>
+      </c>
+      <c r="C5">
+        <v>469.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>474.1</v>
+      </c>
+      <c r="B6">
+        <v>480.8</v>
+      </c>
+      <c r="C6">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>185.3</v>
+      </c>
+      <c r="B2">
+        <v>183.8</v>
+      </c>
+      <c r="C2">
+        <v>187.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>184.4</v>
+      </c>
+      <c r="B3">
+        <v>185.3</v>
+      </c>
+      <c r="C3">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>185.7</v>
+      </c>
+      <c r="B4">
+        <v>185.2</v>
+      </c>
+      <c r="C4">
+        <v>188.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>184.3</v>
+      </c>
+      <c r="B5">
+        <v>183.8</v>
+      </c>
+      <c r="C5">
+        <v>187.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>187.3</v>
+      </c>
+      <c r="B6">
+        <v>186</v>
+      </c>
+      <c r="C6">
+        <v>186.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>283.5</v>
+      </c>
+      <c r="B2">
+        <v>286.2</v>
+      </c>
+      <c r="C2">
+        <v>285.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>285.60000000000002</v>
+      </c>
+      <c r="B3">
+        <v>286.5</v>
+      </c>
+      <c r="C3">
+        <v>286.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>286</v>
+      </c>
+      <c r="B4">
+        <v>285.3</v>
+      </c>
+      <c r="C4">
+        <v>285.39999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>285.5</v>
+      </c>
+      <c r="B5">
+        <v>287.2</v>
+      </c>
+      <c r="C5">
+        <v>286.39999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>286.10000000000002</v>
+      </c>
+      <c r="B6">
+        <v>284.89999999999998</v>
+      </c>
+      <c r="C6">
+        <v>286.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -550,7 +898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -637,7 +985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -724,7 +1072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>